<commit_message>
Adding the front and back heading to the card for more flexibility
</commit_message>
<xml_diff>
--- a/FlashCards.xlsx
+++ b/FlashCards.xlsx
@@ -1148,13 +1148,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1166,8 +1168,8 @@
         <v>1</v>
       </c>
       <c r="D1" t="str">
-        <f>CONCATENATE("new card(""", A1, """,""",B1, """),")</f>
-        <v>new card("Alabama","Montgomery"),</v>
+        <f>CONCATENATE("new card(""State:"",""", A1, """,""Capital:"",""",B1, """),")</f>
+        <v>new card("State:","Alabama","Capital:","Montgomery"),</v>
       </c>
       <c r="F1" t="s">
         <v>100</v>
@@ -1181,8 +1183,8 @@
         <v>3</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D50" si="0">CONCATENATE("new card(""", A2, """,""",B2, """),")</f>
-        <v>new card("Alaska","Juneau"),</v>
+        <f t="shared" ref="D2:D50" si="0">CONCATENATE("new card(""State:"",""", A2, """,""Capital:"",""",B2, """),")</f>
+        <v>new card("State:","Alaska","Capital:","Juneau"),</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1194,7 +1196,7 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Arizona","Phoenix"),</v>
+        <v>new card("State:","Arizona","Capital:","Phoenix"),</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1206,7 +1208,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Arkansas","Little Rock"),</v>
+        <v>new card("State:","Arkansas","Capital:","Little Rock"),</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1218,7 +1220,7 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>new card("California","Sacramento"),</v>
+        <v>new card("State:","California","Capital:","Sacramento"),</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1230,7 +1232,7 @@
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Colorado","Denver"),</v>
+        <v>new card("State:","Colorado","Capital:","Denver"),</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1242,7 +1244,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Connecticut","Hartford"),</v>
+        <v>new card("State:","Connecticut","Capital:","Hartford"),</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1254,7 +1256,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Delaware","Dover"),</v>
+        <v>new card("State:","Delaware","Capital:","Dover"),</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1266,7 +1268,7 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Florida","Tallahassee"),</v>
+        <v>new card("State:","Florida","Capital:","Tallahassee"),</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,7 +1280,7 @@
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Georgia","Atlanta"),</v>
+        <v>new card("State:","Georgia","Capital:","Atlanta"),</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1290,7 +1292,7 @@
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Hawaii","Honolulu"),</v>
+        <v>new card("State:","Hawaii","Capital:","Honolulu"),</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1302,7 +1304,7 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Idaho","Boise"),</v>
+        <v>new card("State:","Idaho","Capital:","Boise"),</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1314,7 +1316,7 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Illinois","Springfield"),</v>
+        <v>new card("State:","Illinois","Capital:","Springfield"),</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1326,7 +1328,7 @@
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Indiana","Indianapolis"),</v>
+        <v>new card("State:","Indiana","Capital:","Indianapolis"),</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1338,7 +1340,7 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Iowa","Des Moines"),</v>
+        <v>new card("State:","Iowa","Capital:","Des Moines"),</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1350,7 +1352,7 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Kansas","Topeka"),</v>
+        <v>new card("State:","Kansas","Capital:","Topeka"),</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1362,7 +1364,7 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Kentucky","Frankfort"),</v>
+        <v>new card("State:","Kentucky","Capital:","Frankfort"),</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1374,7 +1376,7 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Louisiana","Baton Rouge"),</v>
+        <v>new card("State:","Louisiana","Capital:","Baton Rouge"),</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1386,7 +1388,7 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Maine","Augusta"),</v>
+        <v>new card("State:","Maine","Capital:","Augusta"),</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1398,7 +1400,7 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Maryland","Annapolis"),</v>
+        <v>new card("State:","Maryland","Capital:","Annapolis"),</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,7 +1412,7 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Massachusetts","Boston"),</v>
+        <v>new card("State:","Massachusetts","Capital:","Boston"),</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1422,7 +1424,7 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Michigan","Lansing"),</v>
+        <v>new card("State:","Michigan","Capital:","Lansing"),</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1434,7 +1436,7 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Minnesota","St. Paul"),</v>
+        <v>new card("State:","Minnesota","Capital:","St. Paul"),</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1446,7 +1448,7 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Mississippi","Jackson"),</v>
+        <v>new card("State:","Mississippi","Capital:","Jackson"),</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,7 +1460,7 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Missouri","Jefferson City"),</v>
+        <v>new card("State:","Missouri","Capital:","Jefferson City"),</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1470,7 +1472,7 @@
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Montana","Helena"),</v>
+        <v>new card("State:","Montana","Capital:","Helena"),</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1482,7 +1484,7 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Nebraska","Lincoln"),</v>
+        <v>new card("State:","Nebraska","Capital:","Lincoln"),</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1494,7 +1496,7 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Nevada","Carson City"),</v>
+        <v>new card("State:","Nevada","Capital:","Carson City"),</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1506,7 +1508,7 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>new card("New Hampshire","Concord"),</v>
+        <v>new card("State:","New Hampshire","Capital:","Concord"),</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,7 +1520,7 @@
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
-        <v>new card("New Jersey","Trenton"),</v>
+        <v>new card("State:","New Jersey","Capital:","Trenton"),</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1530,7 +1532,7 @@
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
-        <v>new card("New Mexico","Santa Fe"),</v>
+        <v>new card("State:","New Mexico","Capital:","Santa Fe"),</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1542,7 +1544,7 @@
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
-        <v>new card("New York","Albany"),</v>
+        <v>new card("State:","New York","Capital:","Albany"),</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1554,7 +1556,7 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>new card("North Carolina","Raleigh"),</v>
+        <v>new card("State:","North Carolina","Capital:","Raleigh"),</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1566,7 +1568,7 @@
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
-        <v>new card("North Dakota","Bismarck"),</v>
+        <v>new card("State:","North Dakota","Capital:","Bismarck"),</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1578,7 +1580,7 @@
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Ohio","Columbus"),</v>
+        <v>new card("State:","Ohio","Capital:","Columbus"),</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,7 +1592,7 @@
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Oklahoma","Oklahoma City"),</v>
+        <v>new card("State:","Oklahoma","Capital:","Oklahoma City"),</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1602,7 +1604,7 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Oregon","Salem"),</v>
+        <v>new card("State:","Oregon","Capital:","Salem"),</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1614,7 +1616,7 @@
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Pennsylvania","Harrisburg"),</v>
+        <v>new card("State:","Pennsylvania","Capital:","Harrisburg"),</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1626,7 +1628,7 @@
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Rhode Island","Providence"),</v>
+        <v>new card("State:","Rhode Island","Capital:","Providence"),</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1638,7 +1640,7 @@
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
-        <v>new card("South Carolina","Columbia"),</v>
+        <v>new card("State:","South Carolina","Capital:","Columbia"),</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1650,7 +1652,7 @@
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
-        <v>new card("South Dakota","Pierre"),</v>
+        <v>new card("State:","South Dakota","Capital:","Pierre"),</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,7 +1664,7 @@
       </c>
       <c r="D42" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Tennessee","Nashville"),</v>
+        <v>new card("State:","Tennessee","Capital:","Nashville"),</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1674,7 +1676,7 @@
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Texas","Austin"),</v>
+        <v>new card("State:","Texas","Capital:","Austin"),</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1686,7 +1688,7 @@
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Utah","Salt Lake City"),</v>
+        <v>new card("State:","Utah","Capital:","Salt Lake City"),</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1698,7 +1700,7 @@
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Vermont","Montpelier"),</v>
+        <v>new card("State:","Vermont","Capital:","Montpelier"),</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,7 +1712,7 @@
       </c>
       <c r="D46" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Virginia","Richmond"),</v>
+        <v>new card("State:","Virginia","Capital:","Richmond"),</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1722,7 +1724,7 @@
       </c>
       <c r="D47" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Washington","Olympia"),</v>
+        <v>new card("State:","Washington","Capital:","Olympia"),</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1734,7 +1736,7 @@
       </c>
       <c r="D48" t="str">
         <f t="shared" si="0"/>
-        <v>new card("West Virginia","Charleston"),</v>
+        <v>new card("State:","West Virginia","Capital:","Charleston"),</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,7 +1748,7 @@
       </c>
       <c r="D49" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Wisconsin","Madison"),</v>
+        <v>new card("State:","Wisconsin","Capital:","Madison"),</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,7 +1760,7 @@
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
-        <v>new card("Wyoming","Cheyenne"),</v>
+        <v>new card("State:","Wyoming","Capital:","Cheyenne"),</v>
       </c>
     </row>
   </sheetData>
@@ -1771,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E144"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,8 +1798,8 @@
         <v>1</v>
       </c>
       <c r="E1" t="str">
-        <f>CONCATENATE("new card(""", A1, " X ", B1, """,""",C1, """),")</f>
-        <v>new card("1 X 1","1"),</v>
+        <f>CONCATENATE("new card(""Question:"",""", A1, " X ", B1, """,""Answer:"",""",C1, """),")</f>
+        <v>new card("Question:","1 X 1","Answer:","1"),</v>
       </c>
       <c r="G1" t="s">
         <v>100</v>
@@ -1815,8 +1817,8 @@
         <v>2</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E65" si="1">CONCATENATE("new card(""", A2, " X ", B2, """,""",C2, """),")</f>
-        <v>new card("1 X 2","2"),</v>
+        <f t="shared" ref="E2:E65" si="1">CONCATENATE("new card(""Question"",""", A2, " X ", B2, """,""Answer"",""",C2, """),")</f>
+        <v>new card("Question","1 X 2","Answer","2"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1832,7 +1834,7 @@
       </c>
       <c r="E3" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 3","3"),</v>
+        <v>new card("Question","1 X 3","Answer","3"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1848,7 +1850,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 4","4"),</v>
+        <v>new card("Question","1 X 4","Answer","4"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1864,7 +1866,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 5","5"),</v>
+        <v>new card("Question","1 X 5","Answer","5"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1880,7 +1882,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 6","6"),</v>
+        <v>new card("Question","1 X 6","Answer","6"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1896,7 +1898,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 7","7"),</v>
+        <v>new card("Question","1 X 7","Answer","7"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1912,7 +1914,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 8","8"),</v>
+        <v>new card("Question","1 X 8","Answer","8"),</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1928,7 +1930,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 9","9"),</v>
+        <v>new card("Question","1 X 9","Answer","9"),</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1944,7 +1946,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 10","10"),</v>
+        <v>new card("Question","1 X 10","Answer","10"),</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1960,7 +1962,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 11","11"),</v>
+        <v>new card("Question","1 X 11","Answer","11"),</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1976,7 +1978,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>new card("1 X 12","12"),</v>
+        <v>new card("Question","1 X 12","Answer","12"),</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1992,7 +1994,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 1","2"),</v>
+        <v>new card("Question","2 X 1","Answer","2"),</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2008,7 +2010,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 2","4"),</v>
+        <v>new card("Question","2 X 2","Answer","4"),</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2024,7 +2026,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 3","6"),</v>
+        <v>new card("Question","2 X 3","Answer","6"),</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2040,7 +2042,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 4","8"),</v>
+        <v>new card("Question","2 X 4","Answer","8"),</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2056,7 +2058,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 5","10"),</v>
+        <v>new card("Question","2 X 5","Answer","10"),</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2072,7 +2074,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 6","12"),</v>
+        <v>new card("Question","2 X 6","Answer","12"),</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2088,7 +2090,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 7","14"),</v>
+        <v>new card("Question","2 X 7","Answer","14"),</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,7 +2106,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 8","16"),</v>
+        <v>new card("Question","2 X 8","Answer","16"),</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2120,7 +2122,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 9","18"),</v>
+        <v>new card("Question","2 X 9","Answer","18"),</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,7 +2138,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 10","20"),</v>
+        <v>new card("Question","2 X 10","Answer","20"),</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2152,7 +2154,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 11","22"),</v>
+        <v>new card("Question","2 X 11","Answer","22"),</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2168,7 +2170,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>new card("2 X 12","24"),</v>
+        <v>new card("Question","2 X 12","Answer","24"),</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2184,7 +2186,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 1","3"),</v>
+        <v>new card("Question","3 X 1","Answer","3"),</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2200,7 +2202,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 2","6"),</v>
+        <v>new card("Question","3 X 2","Answer","6"),</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2216,7 +2218,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 3","9"),</v>
+        <v>new card("Question","3 X 3","Answer","9"),</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2232,7 +2234,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 4","12"),</v>
+        <v>new card("Question","3 X 4","Answer","12"),</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2248,7 +2250,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 5","15"),</v>
+        <v>new card("Question","3 X 5","Answer","15"),</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2264,7 +2266,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 6","18"),</v>
+        <v>new card("Question","3 X 6","Answer","18"),</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2280,7 +2282,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 7","21"),</v>
+        <v>new card("Question","3 X 7","Answer","21"),</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2296,7 +2298,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 8","24"),</v>
+        <v>new card("Question","3 X 8","Answer","24"),</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2312,7 +2314,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 9","27"),</v>
+        <v>new card("Question","3 X 9","Answer","27"),</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2328,7 +2330,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 10","30"),</v>
+        <v>new card("Question","3 X 10","Answer","30"),</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2344,7 +2346,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 11","33"),</v>
+        <v>new card("Question","3 X 11","Answer","33"),</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2360,7 +2362,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>new card("3 X 12","36"),</v>
+        <v>new card("Question","3 X 12","Answer","36"),</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2376,7 +2378,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 1","4"),</v>
+        <v>new card("Question","4 X 1","Answer","4"),</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2392,7 +2394,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 2","8"),</v>
+        <v>new card("Question","4 X 2","Answer","8"),</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2408,7 +2410,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 3","12"),</v>
+        <v>new card("Question","4 X 3","Answer","12"),</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2424,7 +2426,7 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 4","16"),</v>
+        <v>new card("Question","4 X 4","Answer","16"),</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2440,7 +2442,7 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 5","20"),</v>
+        <v>new card("Question","4 X 5","Answer","20"),</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2456,7 +2458,7 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 6","24"),</v>
+        <v>new card("Question","4 X 6","Answer","24"),</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2472,7 +2474,7 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 7","28"),</v>
+        <v>new card("Question","4 X 7","Answer","28"),</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,7 +2490,7 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 8","32"),</v>
+        <v>new card("Question","4 X 8","Answer","32"),</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2504,7 +2506,7 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 9","36"),</v>
+        <v>new card("Question","4 X 9","Answer","36"),</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2520,7 +2522,7 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 10","40"),</v>
+        <v>new card("Question","4 X 10","Answer","40"),</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2536,7 +2538,7 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 11","44"),</v>
+        <v>new card("Question","4 X 11","Answer","44"),</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2552,7 +2554,7 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>new card("4 X 12","48"),</v>
+        <v>new card("Question","4 X 12","Answer","48"),</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2568,7 +2570,7 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 1","5"),</v>
+        <v>new card("Question","5 X 1","Answer","5"),</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2584,7 +2586,7 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 2","10"),</v>
+        <v>new card("Question","5 X 2","Answer","10"),</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2600,7 +2602,7 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 3","15"),</v>
+        <v>new card("Question","5 X 3","Answer","15"),</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2616,7 +2618,7 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 4","20"),</v>
+        <v>new card("Question","5 X 4","Answer","20"),</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2632,7 +2634,7 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 5","25"),</v>
+        <v>new card("Question","5 X 5","Answer","25"),</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2648,7 +2650,7 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 6","30"),</v>
+        <v>new card("Question","5 X 6","Answer","30"),</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2664,7 +2666,7 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 7","35"),</v>
+        <v>new card("Question","5 X 7","Answer","35"),</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2680,7 +2682,7 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 8","40"),</v>
+        <v>new card("Question","5 X 8","Answer","40"),</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2696,7 +2698,7 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 9","45"),</v>
+        <v>new card("Question","5 X 9","Answer","45"),</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2712,7 +2714,7 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 10","50"),</v>
+        <v>new card("Question","5 X 10","Answer","50"),</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2728,7 +2730,7 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 11","55"),</v>
+        <v>new card("Question","5 X 11","Answer","55"),</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2744,7 +2746,7 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="1"/>
-        <v>new card("5 X 12","60"),</v>
+        <v>new card("Question","5 X 12","Answer","60"),</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2760,7 +2762,7 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="1"/>
-        <v>new card("6 X 1","6"),</v>
+        <v>new card("Question","6 X 1","Answer","6"),</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2776,7 +2778,7 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="1"/>
-        <v>new card("6 X 2","12"),</v>
+        <v>new card("Question","6 X 2","Answer","12"),</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2792,7 +2794,7 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="1"/>
-        <v>new card("6 X 3","18"),</v>
+        <v>new card("Question","6 X 3","Answer","18"),</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2808,7 +2810,7 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="1"/>
-        <v>new card("6 X 4","24"),</v>
+        <v>new card("Question","6 X 4","Answer","24"),</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2824,7 +2826,7 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
-        <v>new card("6 X 5","30"),</v>
+        <v>new card("Question","6 X 5","Answer","30"),</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2839,8 +2841,8 @@
         <v>36</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E129" si="3">CONCATENATE("new card(""", A66, " X ", B66, """,""",C66, """),")</f>
-        <v>new card("6 X 6","36"),</v>
+        <f t="shared" ref="E66:E129" si="3">CONCATENATE("new card(""Question"",""", A66, " X ", B66, """,""Answer"",""",C66, """),")</f>
+        <v>new card("Question","6 X 6","Answer","36"),</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2856,7 +2858,7 @@
       </c>
       <c r="E67" t="str">
         <f t="shared" si="3"/>
-        <v>new card("6 X 7","42"),</v>
+        <v>new card("Question","6 X 7","Answer","42"),</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2872,7 +2874,7 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="3"/>
-        <v>new card("6 X 8","48"),</v>
+        <v>new card("Question","6 X 8","Answer","48"),</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2888,7 +2890,7 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="3"/>
-        <v>new card("6 X 9","54"),</v>
+        <v>new card("Question","6 X 9","Answer","54"),</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2904,7 +2906,7 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="3"/>
-        <v>new card("6 X 10","60"),</v>
+        <v>new card("Question","6 X 10","Answer","60"),</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2920,7 +2922,7 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="3"/>
-        <v>new card("6 X 11","66"),</v>
+        <v>new card("Question","6 X 11","Answer","66"),</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2936,7 +2938,7 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="3"/>
-        <v>new card("6 X 12","72"),</v>
+        <v>new card("Question","6 X 12","Answer","72"),</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2952,7 +2954,7 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 1","7"),</v>
+        <v>new card("Question","7 X 1","Answer","7"),</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2968,7 +2970,7 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 2","14"),</v>
+        <v>new card("Question","7 X 2","Answer","14"),</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2984,7 +2986,7 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 3","21"),</v>
+        <v>new card("Question","7 X 3","Answer","21"),</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3000,7 +3002,7 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 4","28"),</v>
+        <v>new card("Question","7 X 4","Answer","28"),</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3016,7 +3018,7 @@
       </c>
       <c r="E77" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 5","35"),</v>
+        <v>new card("Question","7 X 5","Answer","35"),</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,7 +3034,7 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 6","42"),</v>
+        <v>new card("Question","7 X 6","Answer","42"),</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3048,7 +3050,7 @@
       </c>
       <c r="E79" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 7","49"),</v>
+        <v>new card("Question","7 X 7","Answer","49"),</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3064,7 +3066,7 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 8","56"),</v>
+        <v>new card("Question","7 X 8","Answer","56"),</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3080,7 +3082,7 @@
       </c>
       <c r="E81" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 9","63"),</v>
+        <v>new card("Question","7 X 9","Answer","63"),</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3096,7 +3098,7 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 10","70"),</v>
+        <v>new card("Question","7 X 10","Answer","70"),</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3112,7 +3114,7 @@
       </c>
       <c r="E83" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 11","77"),</v>
+        <v>new card("Question","7 X 11","Answer","77"),</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3128,7 +3130,7 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="3"/>
-        <v>new card("7 X 12","84"),</v>
+        <v>new card("Question","7 X 12","Answer","84"),</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3144,7 +3146,7 @@
       </c>
       <c r="E85" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 1","8"),</v>
+        <v>new card("Question","8 X 1","Answer","8"),</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3160,7 +3162,7 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 2","16"),</v>
+        <v>new card("Question","8 X 2","Answer","16"),</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3176,7 +3178,7 @@
       </c>
       <c r="E87" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 3","24"),</v>
+        <v>new card("Question","8 X 3","Answer","24"),</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3192,7 +3194,7 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 4","32"),</v>
+        <v>new card("Question","8 X 4","Answer","32"),</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3208,7 +3210,7 @@
       </c>
       <c r="E89" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 5","40"),</v>
+        <v>new card("Question","8 X 5","Answer","40"),</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3224,7 +3226,7 @@
       </c>
       <c r="E90" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 6","48"),</v>
+        <v>new card("Question","8 X 6","Answer","48"),</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3240,7 +3242,7 @@
       </c>
       <c r="E91" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 7","56"),</v>
+        <v>new card("Question","8 X 7","Answer","56"),</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3256,7 +3258,7 @@
       </c>
       <c r="E92" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 8","64"),</v>
+        <v>new card("Question","8 X 8","Answer","64"),</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3272,7 +3274,7 @@
       </c>
       <c r="E93" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 9","72"),</v>
+        <v>new card("Question","8 X 9","Answer","72"),</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3288,7 +3290,7 @@
       </c>
       <c r="E94" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 10","80"),</v>
+        <v>new card("Question","8 X 10","Answer","80"),</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3304,7 +3306,7 @@
       </c>
       <c r="E95" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 11","88"),</v>
+        <v>new card("Question","8 X 11","Answer","88"),</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3320,7 +3322,7 @@
       </c>
       <c r="E96" t="str">
         <f t="shared" si="3"/>
-        <v>new card("8 X 12","96"),</v>
+        <v>new card("Question","8 X 12","Answer","96"),</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3336,7 +3338,7 @@
       </c>
       <c r="E97" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 1","9"),</v>
+        <v>new card("Question","9 X 1","Answer","9"),</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3352,7 +3354,7 @@
       </c>
       <c r="E98" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 2","18"),</v>
+        <v>new card("Question","9 X 2","Answer","18"),</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3368,7 +3370,7 @@
       </c>
       <c r="E99" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 3","27"),</v>
+        <v>new card("Question","9 X 3","Answer","27"),</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3384,7 +3386,7 @@
       </c>
       <c r="E100" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 4","36"),</v>
+        <v>new card("Question","9 X 4","Answer","36"),</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3400,7 +3402,7 @@
       </c>
       <c r="E101" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 5","45"),</v>
+        <v>new card("Question","9 X 5","Answer","45"),</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3416,7 +3418,7 @@
       </c>
       <c r="E102" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 6","54"),</v>
+        <v>new card("Question","9 X 6","Answer","54"),</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3432,7 +3434,7 @@
       </c>
       <c r="E103" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 7","63"),</v>
+        <v>new card("Question","9 X 7","Answer","63"),</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3448,7 +3450,7 @@
       </c>
       <c r="E104" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 8","72"),</v>
+        <v>new card("Question","9 X 8","Answer","72"),</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3464,7 +3466,7 @@
       </c>
       <c r="E105" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 9","81"),</v>
+        <v>new card("Question","9 X 9","Answer","81"),</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3480,7 +3482,7 @@
       </c>
       <c r="E106" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 10","90"),</v>
+        <v>new card("Question","9 X 10","Answer","90"),</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3496,7 +3498,7 @@
       </c>
       <c r="E107" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 11","99"),</v>
+        <v>new card("Question","9 X 11","Answer","99"),</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3512,7 +3514,7 @@
       </c>
       <c r="E108" t="str">
         <f t="shared" si="3"/>
-        <v>new card("9 X 12","108"),</v>
+        <v>new card("Question","9 X 12","Answer","108"),</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3528,7 +3530,7 @@
       </c>
       <c r="E109" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 1","10"),</v>
+        <v>new card("Question","10 X 1","Answer","10"),</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3544,7 +3546,7 @@
       </c>
       <c r="E110" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 2","20"),</v>
+        <v>new card("Question","10 X 2","Answer","20"),</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3560,7 +3562,7 @@
       </c>
       <c r="E111" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 3","30"),</v>
+        <v>new card("Question","10 X 3","Answer","30"),</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3576,7 +3578,7 @@
       </c>
       <c r="E112" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 4","40"),</v>
+        <v>new card("Question","10 X 4","Answer","40"),</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,7 +3594,7 @@
       </c>
       <c r="E113" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 5","50"),</v>
+        <v>new card("Question","10 X 5","Answer","50"),</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3608,7 +3610,7 @@
       </c>
       <c r="E114" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 6","60"),</v>
+        <v>new card("Question","10 X 6","Answer","60"),</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3624,7 +3626,7 @@
       </c>
       <c r="E115" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 7","70"),</v>
+        <v>new card("Question","10 X 7","Answer","70"),</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3640,7 +3642,7 @@
       </c>
       <c r="E116" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 8","80"),</v>
+        <v>new card("Question","10 X 8","Answer","80"),</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3656,7 +3658,7 @@
       </c>
       <c r="E117" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 9","90"),</v>
+        <v>new card("Question","10 X 9","Answer","90"),</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3672,7 +3674,7 @@
       </c>
       <c r="E118" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 10","100"),</v>
+        <v>new card("Question","10 X 10","Answer","100"),</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3688,7 +3690,7 @@
       </c>
       <c r="E119" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 11","110"),</v>
+        <v>new card("Question","10 X 11","Answer","110"),</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,7 +3706,7 @@
       </c>
       <c r="E120" t="str">
         <f t="shared" si="3"/>
-        <v>new card("10 X 12","120"),</v>
+        <v>new card("Question","10 X 12","Answer","120"),</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3720,7 +3722,7 @@
       </c>
       <c r="E121" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 1","11"),</v>
+        <v>new card("Question","11 X 1","Answer","11"),</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,7 +3738,7 @@
       </c>
       <c r="E122" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 2","22"),</v>
+        <v>new card("Question","11 X 2","Answer","22"),</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3752,7 +3754,7 @@
       </c>
       <c r="E123" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 3","33"),</v>
+        <v>new card("Question","11 X 3","Answer","33"),</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3768,7 +3770,7 @@
       </c>
       <c r="E124" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 4","44"),</v>
+        <v>new card("Question","11 X 4","Answer","44"),</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3784,7 +3786,7 @@
       </c>
       <c r="E125" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 5","55"),</v>
+        <v>new card("Question","11 X 5","Answer","55"),</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3800,7 +3802,7 @@
       </c>
       <c r="E126" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 6","66"),</v>
+        <v>new card("Question","11 X 6","Answer","66"),</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3816,7 +3818,7 @@
       </c>
       <c r="E127" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 7","77"),</v>
+        <v>new card("Question","11 X 7","Answer","77"),</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3832,7 +3834,7 @@
       </c>
       <c r="E128" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 8","88"),</v>
+        <v>new card("Question","11 X 8","Answer","88"),</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3848,7 +3850,7 @@
       </c>
       <c r="E129" t="str">
         <f t="shared" si="3"/>
-        <v>new card("11 X 9","99"),</v>
+        <v>new card("Question","11 X 9","Answer","99"),</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3863,8 +3865,8 @@
         <v>110</v>
       </c>
       <c r="E130" t="str">
-        <f t="shared" ref="E130:E144" si="5">CONCATENATE("new card(""", A130, " X ", B130, """,""",C130, """),")</f>
-        <v>new card("11 X 10","110"),</v>
+        <f t="shared" ref="E130:E144" si="5">CONCATENATE("new card(""Question"",""", A130, " X ", B130, """,""Answer"",""",C130, """),")</f>
+        <v>new card("Question","11 X 10","Answer","110"),</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3880,7 +3882,7 @@
       </c>
       <c r="E131" t="str">
         <f t="shared" si="5"/>
-        <v>new card("11 X 11","121"),</v>
+        <v>new card("Question","11 X 11","Answer","121"),</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3896,7 +3898,7 @@
       </c>
       <c r="E132" t="str">
         <f t="shared" si="5"/>
-        <v>new card("11 X 12","132"),</v>
+        <v>new card("Question","11 X 12","Answer","132"),</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3912,7 +3914,7 @@
       </c>
       <c r="E133" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 1","12"),</v>
+        <v>new card("Question","12 X 1","Answer","12"),</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3928,7 +3930,7 @@
       </c>
       <c r="E134" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 2","24"),</v>
+        <v>new card("Question","12 X 2","Answer","24"),</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3944,7 +3946,7 @@
       </c>
       <c r="E135" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 3","36"),</v>
+        <v>new card("Question","12 X 3","Answer","36"),</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3960,7 +3962,7 @@
       </c>
       <c r="E136" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 4","48"),</v>
+        <v>new card("Question","12 X 4","Answer","48"),</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3976,7 +3978,7 @@
       </c>
       <c r="E137" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 5","60"),</v>
+        <v>new card("Question","12 X 5","Answer","60"),</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3992,7 +3994,7 @@
       </c>
       <c r="E138" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 6","72"),</v>
+        <v>new card("Question","12 X 6","Answer","72"),</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4008,7 +4010,7 @@
       </c>
       <c r="E139" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 7","84"),</v>
+        <v>new card("Question","12 X 7","Answer","84"),</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4024,7 +4026,7 @@
       </c>
       <c r="E140" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 8","96"),</v>
+        <v>new card("Question","12 X 8","Answer","96"),</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4040,7 +4042,7 @@
       </c>
       <c r="E141" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 9","108"),</v>
+        <v>new card("Question","12 X 9","Answer","108"),</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4056,7 +4058,7 @@
       </c>
       <c r="E142" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 10","120"),</v>
+        <v>new card("Question","12 X 10","Answer","120"),</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4072,7 +4074,7 @@
       </c>
       <c r="E143" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 11","132"),</v>
+        <v>new card("Question","12 X 11","Answer","132"),</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4088,7 +4090,7 @@
       </c>
       <c r="E144" t="str">
         <f t="shared" si="5"/>
-        <v>new card("12 X 12","144"),</v>
+        <v>new card("Question","12 X 12","Answer","144"),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the multiplication data
</commit_message>
<xml_diff>
--- a/FlashCards.xlsx
+++ b/FlashCards.xlsx
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,8 +1817,8 @@
         <v>2</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E65" si="1">CONCATENATE("new card(""Question"",""", A2, " X ", B2, """,""Answer"",""",C2, """),")</f>
-        <v>new card("Question","1 X 2","Answer","2"),</v>
+        <f t="shared" ref="E2:E65" si="1">CONCATENATE("new card(""Question:"",""", A2, " X ", B2, """,""Answer:"",""",C2, """),")</f>
+        <v>new card("Question:","1 X 2","Answer:","2"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="E3" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 3","Answer","3"),</v>
+        <v>new card("Question:","1 X 3","Answer:","3"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 4","Answer","4"),</v>
+        <v>new card("Question:","1 X 4","Answer:","4"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 5","Answer","5"),</v>
+        <v>new card("Question:","1 X 5","Answer:","5"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 6","Answer","6"),</v>
+        <v>new card("Question:","1 X 6","Answer:","6"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1898,7 +1898,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 7","Answer","7"),</v>
+        <v>new card("Question:","1 X 7","Answer:","7"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 8","Answer","8"),</v>
+        <v>new card("Question:","1 X 8","Answer:","8"),</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1930,7 +1930,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 9","Answer","9"),</v>
+        <v>new card("Question:","1 X 9","Answer:","9"),</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 10","Answer","10"),</v>
+        <v>new card("Question:","1 X 10","Answer:","10"),</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1962,7 +1962,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 11","Answer","11"),</v>
+        <v>new card("Question:","1 X 11","Answer:","11"),</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","1 X 12","Answer","12"),</v>
+        <v>new card("Question:","1 X 12","Answer:","12"),</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 1","Answer","2"),</v>
+        <v>new card("Question:","2 X 1","Answer:","2"),</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 2","Answer","4"),</v>
+        <v>new card("Question:","2 X 2","Answer:","4"),</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 3","Answer","6"),</v>
+        <v>new card("Question:","2 X 3","Answer:","6"),</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 4","Answer","8"),</v>
+        <v>new card("Question:","2 X 4","Answer:","8"),</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2058,7 +2058,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 5","Answer","10"),</v>
+        <v>new card("Question:","2 X 5","Answer:","10"),</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,7 +2074,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 6","Answer","12"),</v>
+        <v>new card("Question:","2 X 6","Answer:","12"),</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 7","Answer","14"),</v>
+        <v>new card("Question:","2 X 7","Answer:","14"),</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2106,7 +2106,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 8","Answer","16"),</v>
+        <v>new card("Question:","2 X 8","Answer:","16"),</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 9","Answer","18"),</v>
+        <v>new card("Question:","2 X 9","Answer:","18"),</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 10","Answer","20"),</v>
+        <v>new card("Question:","2 X 10","Answer:","20"),</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 11","Answer","22"),</v>
+        <v>new card("Question:","2 X 11","Answer:","22"),</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","2 X 12","Answer","24"),</v>
+        <v>new card("Question:","2 X 12","Answer:","24"),</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2186,7 +2186,7 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 1","Answer","3"),</v>
+        <v>new card("Question:","3 X 1","Answer:","3"),</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 2","Answer","6"),</v>
+        <v>new card("Question:","3 X 2","Answer:","6"),</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2218,7 +2218,7 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 3","Answer","9"),</v>
+        <v>new card("Question:","3 X 3","Answer:","9"),</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 4","Answer","12"),</v>
+        <v>new card("Question:","3 X 4","Answer:","12"),</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2250,7 +2250,7 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 5","Answer","15"),</v>
+        <v>new card("Question:","3 X 5","Answer:","15"),</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 6","Answer","18"),</v>
+        <v>new card("Question:","3 X 6","Answer:","18"),</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 7","Answer","21"),</v>
+        <v>new card("Question:","3 X 7","Answer:","21"),</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 8","Answer","24"),</v>
+        <v>new card("Question:","3 X 8","Answer:","24"),</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 9","Answer","27"),</v>
+        <v>new card("Question:","3 X 9","Answer:","27"),</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2330,7 +2330,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 10","Answer","30"),</v>
+        <v>new card("Question:","3 X 10","Answer:","30"),</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 11","Answer","33"),</v>
+        <v>new card("Question:","3 X 11","Answer:","33"),</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","3 X 12","Answer","36"),</v>
+        <v>new card("Question:","3 X 12","Answer:","36"),</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 1","Answer","4"),</v>
+        <v>new card("Question:","4 X 1","Answer:","4"),</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2394,7 +2394,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 2","Answer","8"),</v>
+        <v>new card("Question:","4 X 2","Answer:","8"),</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 3","Answer","12"),</v>
+        <v>new card("Question:","4 X 3","Answer:","12"),</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 4","Answer","16"),</v>
+        <v>new card("Question:","4 X 4","Answer:","16"),</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2442,7 +2442,7 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 5","Answer","20"),</v>
+        <v>new card("Question:","4 X 5","Answer:","20"),</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 6","Answer","24"),</v>
+        <v>new card("Question:","4 X 6","Answer:","24"),</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2474,7 +2474,7 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 7","Answer","28"),</v>
+        <v>new card("Question:","4 X 7","Answer:","28"),</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2490,7 +2490,7 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 8","Answer","32"),</v>
+        <v>new card("Question:","4 X 8","Answer:","32"),</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 9","Answer","36"),</v>
+        <v>new card("Question:","4 X 9","Answer:","36"),</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2522,7 +2522,7 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 10","Answer","40"),</v>
+        <v>new card("Question:","4 X 10","Answer:","40"),</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 11","Answer","44"),</v>
+        <v>new card("Question:","4 X 11","Answer:","44"),</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","4 X 12","Answer","48"),</v>
+        <v>new card("Question:","4 X 12","Answer:","48"),</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2570,7 +2570,7 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 1","Answer","5"),</v>
+        <v>new card("Question:","5 X 1","Answer:","5"),</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2586,7 +2586,7 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 2","Answer","10"),</v>
+        <v>new card("Question:","5 X 2","Answer:","10"),</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 3","Answer","15"),</v>
+        <v>new card("Question:","5 X 3","Answer:","15"),</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 4","Answer","20"),</v>
+        <v>new card("Question:","5 X 4","Answer:","20"),</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 5","Answer","25"),</v>
+        <v>new card("Question:","5 X 5","Answer:","25"),</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2650,7 +2650,7 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 6","Answer","30"),</v>
+        <v>new card("Question:","5 X 6","Answer:","30"),</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 7","Answer","35"),</v>
+        <v>new card("Question:","5 X 7","Answer:","35"),</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 8","Answer","40"),</v>
+        <v>new card("Question:","5 X 8","Answer:","40"),</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2698,7 +2698,7 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 9","Answer","45"),</v>
+        <v>new card("Question:","5 X 9","Answer:","45"),</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 10","Answer","50"),</v>
+        <v>new card("Question:","5 X 10","Answer:","50"),</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2730,7 +2730,7 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 11","Answer","55"),</v>
+        <v>new card("Question:","5 X 11","Answer:","55"),</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","5 X 12","Answer","60"),</v>
+        <v>new card("Question:","5 X 12","Answer:","60"),</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","6 X 1","Answer","6"),</v>
+        <v>new card("Question:","6 X 1","Answer:","6"),</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","6 X 2","Answer","12"),</v>
+        <v>new card("Question:","6 X 2","Answer:","12"),</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","6 X 3","Answer","18"),</v>
+        <v>new card("Question:","6 X 3","Answer:","18"),</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2810,7 +2810,7 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","6 X 4","Answer","24"),</v>
+        <v>new card("Question:","6 X 4","Answer:","24"),</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
-        <v>new card("Question","6 X 5","Answer","30"),</v>
+        <v>new card("Question:","6 X 5","Answer:","30"),</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2841,8 +2841,8 @@
         <v>36</v>
       </c>
       <c r="E66" t="str">
-        <f t="shared" ref="E66:E129" si="3">CONCATENATE("new card(""Question"",""", A66, " X ", B66, """,""Answer"",""",C66, """),")</f>
-        <v>new card("Question","6 X 6","Answer","36"),</v>
+        <f t="shared" ref="E66:E129" si="3">CONCATENATE("new card(""Question:"",""", A66, " X ", B66, """,""Answer:"",""",C66, """),")</f>
+        <v>new card("Question:","6 X 6","Answer:","36"),</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="E67" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","6 X 7","Answer","42"),</v>
+        <v>new card("Question:","6 X 7","Answer:","42"),</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2874,7 +2874,7 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","6 X 8","Answer","48"),</v>
+        <v>new card("Question:","6 X 8","Answer:","48"),</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","6 X 9","Answer","54"),</v>
+        <v>new card("Question:","6 X 9","Answer:","54"),</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","6 X 10","Answer","60"),</v>
+        <v>new card("Question:","6 X 10","Answer:","60"),</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","6 X 11","Answer","66"),</v>
+        <v>new card("Question:","6 X 11","Answer:","66"),</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","6 X 12","Answer","72"),</v>
+        <v>new card("Question:","6 X 12","Answer:","72"),</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 1","Answer","7"),</v>
+        <v>new card("Question:","7 X 1","Answer:","7"),</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 2","Answer","14"),</v>
+        <v>new card("Question:","7 X 2","Answer:","14"),</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 3","Answer","21"),</v>
+        <v>new card("Question:","7 X 3","Answer:","21"),</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 4","Answer","28"),</v>
+        <v>new card("Question:","7 X 4","Answer:","28"),</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
       </c>
       <c r="E77" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 5","Answer","35"),</v>
+        <v>new card("Question:","7 X 5","Answer:","35"),</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 6","Answer","42"),</v>
+        <v>new card("Question:","7 X 6","Answer:","42"),</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3050,7 +3050,7 @@
       </c>
       <c r="E79" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 7","Answer","49"),</v>
+        <v>new card("Question:","7 X 7","Answer:","49"),</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 8","Answer","56"),</v>
+        <v>new card("Question:","7 X 8","Answer:","56"),</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3082,7 +3082,7 @@
       </c>
       <c r="E81" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 9","Answer","63"),</v>
+        <v>new card("Question:","7 X 9","Answer:","63"),</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 10","Answer","70"),</v>
+        <v>new card("Question:","7 X 10","Answer:","70"),</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3114,7 +3114,7 @@
       </c>
       <c r="E83" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 11","Answer","77"),</v>
+        <v>new card("Question:","7 X 11","Answer:","77"),</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","7 X 12","Answer","84"),</v>
+        <v>new card("Question:","7 X 12","Answer:","84"),</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="E85" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 1","Answer","8"),</v>
+        <v>new card("Question:","8 X 1","Answer:","8"),</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 2","Answer","16"),</v>
+        <v>new card("Question:","8 X 2","Answer:","16"),</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3178,7 +3178,7 @@
       </c>
       <c r="E87" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 3","Answer","24"),</v>
+        <v>new card("Question:","8 X 3","Answer:","24"),</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 4","Answer","32"),</v>
+        <v>new card("Question:","8 X 4","Answer:","32"),</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3210,7 +3210,7 @@
       </c>
       <c r="E89" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 5","Answer","40"),</v>
+        <v>new card("Question:","8 X 5","Answer:","40"),</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3226,7 +3226,7 @@
       </c>
       <c r="E90" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 6","Answer","48"),</v>
+        <v>new card("Question:","8 X 6","Answer:","48"),</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3242,7 +3242,7 @@
       </c>
       <c r="E91" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 7","Answer","56"),</v>
+        <v>new card("Question:","8 X 7","Answer:","56"),</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="E92" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 8","Answer","64"),</v>
+        <v>new card("Question:","8 X 8","Answer:","64"),</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="E93" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 9","Answer","72"),</v>
+        <v>new card("Question:","8 X 9","Answer:","72"),</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3290,7 +3290,7 @@
       </c>
       <c r="E94" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 10","Answer","80"),</v>
+        <v>new card("Question:","8 X 10","Answer:","80"),</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -3306,7 +3306,7 @@
       </c>
       <c r="E95" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 11","Answer","88"),</v>
+        <v>new card("Question:","8 X 11","Answer:","88"),</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="E96" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","8 X 12","Answer","96"),</v>
+        <v>new card("Question:","8 X 12","Answer:","96"),</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -3338,7 +3338,7 @@
       </c>
       <c r="E97" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 1","Answer","9"),</v>
+        <v>new card("Question:","9 X 1","Answer:","9"),</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3354,7 +3354,7 @@
       </c>
       <c r="E98" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 2","Answer","18"),</v>
+        <v>new card("Question:","9 X 2","Answer:","18"),</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="E99" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 3","Answer","27"),</v>
+        <v>new card("Question:","9 X 3","Answer:","27"),</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="E100" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 4","Answer","36"),</v>
+        <v>new card("Question:","9 X 4","Answer:","36"),</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="E101" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 5","Answer","45"),</v>
+        <v>new card("Question:","9 X 5","Answer:","45"),</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
       </c>
       <c r="E102" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 6","Answer","54"),</v>
+        <v>new card("Question:","9 X 6","Answer:","54"),</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -3434,7 +3434,7 @@
       </c>
       <c r="E103" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 7","Answer","63"),</v>
+        <v>new card("Question:","9 X 7","Answer:","63"),</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="E104" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 8","Answer","72"),</v>
+        <v>new card("Question:","9 X 8","Answer:","72"),</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="E105" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 9","Answer","81"),</v>
+        <v>new card("Question:","9 X 9","Answer:","81"),</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -3482,7 +3482,7 @@
       </c>
       <c r="E106" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 10","Answer","90"),</v>
+        <v>new card("Question:","9 X 10","Answer:","90"),</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -3498,7 +3498,7 @@
       </c>
       <c r="E107" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 11","Answer","99"),</v>
+        <v>new card("Question:","9 X 11","Answer:","99"),</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -3514,7 +3514,7 @@
       </c>
       <c r="E108" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","9 X 12","Answer","108"),</v>
+        <v>new card("Question:","9 X 12","Answer:","108"),</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="E109" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 1","Answer","10"),</v>
+        <v>new card("Question:","10 X 1","Answer:","10"),</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
       </c>
       <c r="E110" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 2","Answer","20"),</v>
+        <v>new card("Question:","10 X 2","Answer:","20"),</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3562,7 +3562,7 @@
       </c>
       <c r="E111" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 3","Answer","30"),</v>
+        <v>new card("Question:","10 X 3","Answer:","30"),</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E112" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 4","Answer","40"),</v>
+        <v>new card("Question:","10 X 4","Answer:","40"),</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="E113" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 5","Answer","50"),</v>
+        <v>new card("Question:","10 X 5","Answer:","50"),</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="E114" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 6","Answer","60"),</v>
+        <v>new card("Question:","10 X 6","Answer:","60"),</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="E115" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 7","Answer","70"),</v>
+        <v>new card("Question:","10 X 7","Answer:","70"),</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3642,7 +3642,7 @@
       </c>
       <c r="E116" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 8","Answer","80"),</v>
+        <v>new card("Question:","10 X 8","Answer:","80"),</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="E117" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 9","Answer","90"),</v>
+        <v>new card("Question:","10 X 9","Answer:","90"),</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="E118" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 10","Answer","100"),</v>
+        <v>new card("Question:","10 X 10","Answer:","100"),</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E119" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 11","Answer","110"),</v>
+        <v>new card("Question:","10 X 11","Answer:","110"),</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="E120" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","10 X 12","Answer","120"),</v>
+        <v>new card("Question:","10 X 12","Answer:","120"),</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="E121" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 1","Answer","11"),</v>
+        <v>new card("Question:","11 X 1","Answer:","11"),</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3738,7 +3738,7 @@
       </c>
       <c r="E122" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 2","Answer","22"),</v>
+        <v>new card("Question:","11 X 2","Answer:","22"),</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3754,7 +3754,7 @@
       </c>
       <c r="E123" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 3","Answer","33"),</v>
+        <v>new card("Question:","11 X 3","Answer:","33"),</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3770,7 +3770,7 @@
       </c>
       <c r="E124" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 4","Answer","44"),</v>
+        <v>new card("Question:","11 X 4","Answer:","44"),</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="E125" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 5","Answer","55"),</v>
+        <v>new card("Question:","11 X 5","Answer:","55"),</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3802,7 +3802,7 @@
       </c>
       <c r="E126" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 6","Answer","66"),</v>
+        <v>new card("Question:","11 X 6","Answer:","66"),</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="E127" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 7","Answer","77"),</v>
+        <v>new card("Question:","11 X 7","Answer:","77"),</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3834,7 +3834,7 @@
       </c>
       <c r="E128" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 8","Answer","88"),</v>
+        <v>new card("Question:","11 X 8","Answer:","88"),</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3850,7 +3850,7 @@
       </c>
       <c r="E129" t="str">
         <f t="shared" si="3"/>
-        <v>new card("Question","11 X 9","Answer","99"),</v>
+        <v>new card("Question:","11 X 9","Answer:","99"),</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3865,8 +3865,8 @@
         <v>110</v>
       </c>
       <c r="E130" t="str">
-        <f t="shared" ref="E130:E144" si="5">CONCATENATE("new card(""Question"",""", A130, " X ", B130, """,""Answer"",""",C130, """),")</f>
-        <v>new card("Question","11 X 10","Answer","110"),</v>
+        <f t="shared" ref="E130:E144" si="5">CONCATENATE("new card(""Question:"",""", A130, " X ", B130, """,""Answer:"",""",C130, """),")</f>
+        <v>new card("Question:","11 X 10","Answer:","110"),</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3882,7 +3882,7 @@
       </c>
       <c r="E131" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","11 X 11","Answer","121"),</v>
+        <v>new card("Question:","11 X 11","Answer:","121"),</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="E132" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","11 X 12","Answer","132"),</v>
+        <v>new card("Question:","11 X 12","Answer:","132"),</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3914,7 +3914,7 @@
       </c>
       <c r="E133" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 1","Answer","12"),</v>
+        <v>new card("Question:","12 X 1","Answer:","12"),</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3930,7 +3930,7 @@
       </c>
       <c r="E134" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 2","Answer","24"),</v>
+        <v>new card("Question:","12 X 2","Answer:","24"),</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3946,7 +3946,7 @@
       </c>
       <c r="E135" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 3","Answer","36"),</v>
+        <v>new card("Question:","12 X 3","Answer:","36"),</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3962,7 +3962,7 @@
       </c>
       <c r="E136" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 4","Answer","48"),</v>
+        <v>new card("Question:","12 X 4","Answer:","48"),</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="E137" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 5","Answer","60"),</v>
+        <v>new card("Question:","12 X 5","Answer:","60"),</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3994,7 +3994,7 @@
       </c>
       <c r="E138" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 6","Answer","72"),</v>
+        <v>new card("Question:","12 X 6","Answer:","72"),</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4010,7 +4010,7 @@
       </c>
       <c r="E139" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 7","Answer","84"),</v>
+        <v>new card("Question:","12 X 7","Answer:","84"),</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="E140" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 8","Answer","96"),</v>
+        <v>new card("Question:","12 X 8","Answer:","96"),</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4042,7 +4042,7 @@
       </c>
       <c r="E141" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 9","Answer","108"),</v>
+        <v>new card("Question:","12 X 9","Answer:","108"),</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="E142" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 10","Answer","120"),</v>
+        <v>new card("Question:","12 X 10","Answer:","120"),</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4074,7 +4074,7 @@
       </c>
       <c r="E143" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 11","Answer","132"),</v>
+        <v>new card("Question:","12 X 11","Answer:","132"),</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4090,7 +4090,7 @@
       </c>
       <c r="E144" t="str">
         <f t="shared" si="5"/>
-        <v>new card("Question","12 X 12","Answer","144"),</v>
+        <v>new card("Question:","12 X 12","Answer:","144"),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>